<commit_message>
fix credit_account in supplier managemnet
</commit_message>
<xml_diff>
--- a/input_invoices.xlsx
+++ b/input_invoices.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\original\invoices-to-journal-entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F283A2-4379-45EE-A64A-06E9242D2CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0025254C-187F-4940-AC03-4E0BA7DCD796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0A13CA94-C18A-4954-A2E1-975EA8B9F1AC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="13">
   <si>
     <t>رقم الفاتورة</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>الامام2</t>
+  </si>
+  <si>
+    <t>مورد1</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -167,7 +170,10 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -211,7 +217,7 @@
       <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -223,19 +229,10 @@
       <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -255,17 +252,17 @@
   <autoFilter ref="A1:H24" xr:uid="{D1DB59FA-8479-4309-8685-758AFAF8A911}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F20D9A04-3B88-4687-80FF-52723F7500F0}" name="التاريخ"/>
-    <tableColumn id="6" xr3:uid="{E3F71AF4-E980-4E2C-9BED-236EFCBE7903}" name="اصل المبلغ" dataDxfId="13" totalsRowDxfId="9" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{1DA8725E-1FB9-4267-BD7C-4F28632287CB}" name="الضريبة" dataDxfId="12" totalsRowDxfId="8" dataCellStyle="Comma">
+    <tableColumn id="6" xr3:uid="{E3F71AF4-E980-4E2C-9BED-236EFCBE7903}" name="اصل المبلغ" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{1DA8725E-1FB9-4267-BD7C-4F28632287CB}" name="الضريبة" dataDxfId="10" totalsRowDxfId="9" dataCellStyle="Comma">
       <calculatedColumnFormula>B2*0.15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{75620BB7-93CA-4F2F-ACE1-DDC66C9CC8B7}" name="المبلغ شامل الضريبة" dataDxfId="11" totalsRowDxfId="7" dataCellStyle="Comma">
+    <tableColumn id="8" xr3:uid="{75620BB7-93CA-4F2F-ACE1-DDC66C9CC8B7}" name="المبلغ شامل الضريبة" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Comma">
       <calculatedColumnFormula>C2+B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4AFBE490-69AC-4DBB-8471-9DDF81CEE836}" name="المشروع" dataDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="2" xr3:uid="{941E0EA6-B6A3-48E3-AB84-BF66FAC4BA34}" name="رقم الفاتورة" dataDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{4AFBE490-69AC-4DBB-8471-9DDF81CEE836}" name="المشروع" dataDxfId="6" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{941E0EA6-B6A3-48E3-AB84-BF66FAC4BA34}" name="رقم الفاتورة" dataDxfId="5" dataCellStyle="Comma"/>
     <tableColumn id="3" xr3:uid="{4E79DF70-4C49-46F6-A95E-886D604D3B9A}" name="المورد"/>
-    <tableColumn id="4" xr3:uid="{2605E4A4-BC9F-447E-996B-A46A0DB7EA6A}" name="الرقم الضريبي" dataDxfId="10" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{2605E4A4-BC9F-447E-996B-A46A0DB7EA6A}" name="الرقم الضريبي" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -574,7 +571,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,10 +637,10 @@
         <v>5463</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2">
-        <v>310169565400003</v>
+        <v>3100000000003</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>